<commit_message>
column 3 changed to  index-Rvar1
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_rProductLanding.xlsx
+++ b/docs/OVW Sheets/OVWDemo_rProductLanding.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Dec 28\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dec30\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="26" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>routers</t>
   </si>
   <si>
-    <t>rprod_landing-var1</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/JP/product/hs/switches/index.html</t>
   </si>
   <si>
@@ -897,6 +894,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/ZA/products/storage/index.html</t>
+  </si>
+  <si>
+    <t>index-Rvar1</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1287,13 +1287,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1301,13 +1301,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1315,13 +1315,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1329,13 +1329,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" t="s">
         <v>196</v>
-      </c>
-      <c r="B6" t="s">
-        <v>197</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" t="s">
         <v>198</v>
-      </c>
-      <c r="B7" t="s">
-        <v>199</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1397,7 +1397,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,13 +1409,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1423,13 +1423,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1437,13 +1437,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1451,13 +1451,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1465,13 +1465,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1479,10 +1479,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1533,25 +1533,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1559,13 +1559,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1573,13 +1573,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1587,13 +1587,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1601,13 +1601,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1615,10 +1615,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1669,25 +1669,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1695,13 +1695,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1709,13 +1709,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1723,13 +1723,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1805,7 +1805,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,13 +1817,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1831,13 +1831,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1845,13 +1845,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1859,13 +1859,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1873,13 +1873,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1887,10 +1887,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,13 +1953,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1967,13 +1967,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1981,13 +1981,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1995,13 +1995,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2009,13 +2009,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2023,10 +2023,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2077,25 +2077,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2103,13 +2103,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2117,13 +2117,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2131,13 +2131,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2145,13 +2145,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2170,10 +2170,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2213,25 +2213,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2239,13 +2239,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2267,13 +2267,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2281,13 +2281,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2295,10 +2295,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2349,25 +2349,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2375,13 +2375,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2389,13 +2389,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2403,13 +2403,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2417,13 +2417,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2431,10 +2431,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2485,7 +2485,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,13 +2497,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2525,13 +2525,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2553,13 +2553,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2578,10 +2578,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2621,25 +2621,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2661,13 +2661,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2675,13 +2675,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2689,13 +2689,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2703,10 +2703,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2757,26 +2757,26 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2784,13 +2784,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2812,13 +2812,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2827,13 +2827,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2842,10 +2842,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2853,10 +2853,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2881,25 +2881,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2907,13 +2907,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2921,13 +2921,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2935,13 +2935,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2949,13 +2949,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2963,10 +2963,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2974,10 +2974,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3017,25 +3017,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3043,13 +3043,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3057,13 +3057,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3071,13 +3071,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3099,10 +3099,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3110,10 +3110,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3153,25 +3153,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3179,13 +3179,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3193,13 +3193,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3207,13 +3207,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3235,10 +3235,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3246,10 +3246,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3289,25 +3289,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3315,13 +3315,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3329,13 +3329,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3343,13 +3343,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3357,13 +3357,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3371,10 +3371,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3382,10 +3382,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3425,25 +3425,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3451,13 +3451,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3465,13 +3465,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3479,13 +3479,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3493,13 +3493,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3507,10 +3507,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3518,10 +3518,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3561,25 +3561,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3587,13 +3587,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3601,13 +3601,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3615,13 +3615,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3629,13 +3629,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3643,10 +3643,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3697,25 +3697,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3723,13 +3723,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3737,13 +3737,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3765,13 +3765,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3779,10 +3779,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3790,10 +3790,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3833,25 +3833,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3859,13 +3859,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3873,13 +3873,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3887,13 +3887,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3901,13 +3901,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3915,10 +3915,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -3926,10 +3926,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -3969,7 +3969,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,13 +3981,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3995,13 +3995,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4009,13 +4009,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4023,13 +4023,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4037,13 +4037,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4051,10 +4051,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4062,10 +4062,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4105,25 +4105,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4131,13 +4131,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4145,13 +4145,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4159,13 +4159,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4173,13 +4173,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4187,10 +4187,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4198,10 +4198,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4241,7 +4241,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,13 +4253,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4267,13 +4267,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4281,13 +4281,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4295,13 +4295,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4309,13 +4309,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4323,10 +4323,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4377,25 +4377,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4403,13 +4403,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4417,13 +4417,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4431,13 +4431,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4445,13 +4445,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4459,10 +4459,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4470,10 +4470,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4513,7 +4513,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4525,13 +4525,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4539,13 +4539,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4553,13 +4553,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4567,13 +4567,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4581,13 +4581,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4595,10 +4595,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4606,10 +4606,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4649,25 +4649,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4675,13 +4675,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4689,13 +4689,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4703,13 +4703,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4717,13 +4717,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4731,10 +4731,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4742,10 +4742,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4785,25 +4785,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4811,13 +4811,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4825,13 +4825,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4839,13 +4839,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4853,13 +4853,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4867,10 +4867,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4878,10 +4878,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4921,25 +4921,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -4947,13 +4947,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4961,13 +4961,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4975,13 +4975,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4989,13 +4989,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5003,10 +5003,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5014,10 +5014,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5057,25 +5057,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5097,13 +5097,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5111,13 +5111,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5125,13 +5125,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5139,10 +5139,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5150,10 +5150,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5205,10 +5205,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5216,10 +5216,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5239,26 +5239,26 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5266,13 +5266,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5280,13 +5280,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5294,13 +5294,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5308,13 +5308,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5333,10 +5333,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5376,25 +5376,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5402,13 +5402,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5416,13 +5416,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5430,13 +5430,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5444,13 +5444,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5458,10 +5458,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5512,25 +5512,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5538,13 +5538,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5552,13 +5552,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5566,13 +5566,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5580,13 +5580,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5594,10 +5594,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5605,10 +5605,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5647,8 +5647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5660,13 +5660,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5674,13 +5674,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5688,13 +5688,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5702,13 +5702,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5716,13 +5716,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5730,10 +5730,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5741,10 +5741,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5783,26 +5783,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5810,13 +5810,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5824,13 +5824,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5838,13 +5838,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5852,13 +5852,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -5866,10 +5866,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -5877,10 +5877,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -5920,7 +5920,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5932,13 +5932,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5946,13 +5946,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5960,13 +5960,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5974,13 +5974,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -5988,13 +5988,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6002,10 +6002,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -6013,10 +6013,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -6056,26 +6056,26 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6083,13 +6083,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6097,13 +6097,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -6111,13 +6111,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -6126,13 +6126,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6141,10 +6141,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -6152,10 +6152,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -6181,7 +6181,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6194,13 +6194,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6208,13 +6208,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6222,13 +6222,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -6236,13 +6236,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -6251,13 +6251,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6266,10 +6266,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -6277,10 +6277,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -6305,7 +6305,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6318,13 +6318,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6332,13 +6332,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6346,13 +6346,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -6360,13 +6360,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -6375,13 +6375,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6390,10 +6390,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -6401,10 +6401,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -6430,26 +6430,26 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6457,13 +6457,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6471,13 +6471,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -6485,13 +6485,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -6500,13 +6500,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6515,10 +6515,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -6526,10 +6526,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>

</xml_diff>